<commit_message>
Added the planning, finished the plan of attack, added new entries to my log
</commit_message>
<xml_diff>
--- a/Documentation/Logs/log_job.xlsx
+++ b/Documentation/Logs/log_job.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Researching PNG rendering</t>
+  </si>
+  <si>
+    <t>MessageQueue and rendering design, Cutting out tiles</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Plan of Attack</t>
   </si>
 </sst>
 </file>
@@ -404,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -535,6 +544,46 @@
       </c>
       <c r="F6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>40220</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>40225</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated log till 17-3-2010
</commit_message>
<xml_diff>
--- a/Documentation/Logs/log_job.xlsx
+++ b/Documentation/Logs/log_job.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -96,10 +96,25 @@
     <t>Design for level/parallax scrolling + gadgets</t>
   </si>
   <si>
-    <t>Realisation and Desing</t>
-  </si>
-  <si>
     <t>GadgetFactory design and implementation</t>
+  </si>
+  <si>
+    <t>Design multiple kinds of surfaces, enemy implementation</t>
+  </si>
+  <si>
+    <t>Enemy factory</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Tiles for the snow level</t>
+  </si>
+  <si>
+    <t>4.75</t>
+  </si>
+  <si>
+    <t>Snowlevel implementation, all tiles and some surfaces</t>
   </si>
 </sst>
 </file>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -755,11 +770,244 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="F15" t="s">
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>40247</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D16" s="4">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>40248</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>40252</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>40253</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="4:4">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="4:4">
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="4:4">
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="4:4">
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="4:4">
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="4:4">
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="4:4">
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="4:4">
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="4:4">
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="4:4">
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="4:4">
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="4:4">
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="4:4">
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="4:4">
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="4:4">
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="4:4">
+      <c r="D70" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>